<commit_message>
Troca combo por input
</commit_message>
<xml_diff>
--- a/docs/features.xlsx
+++ b/docs/features.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Henrique\repos\fatec\fatecarona\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA6722CE-2C6E-4BEA-954D-5F442BABEBB3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DACB13-A33C-4FE0-8CF9-E05666BE0C8E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="1740" windowWidth="21600" windowHeight="11385" xr2:uid="{DC52FC83-1E62-41CF-BA03-5670C0B62DFB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DC52FC83-1E62-41CF-BA03-5670C0B62DFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -445,7 +445,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Altera todos combo de cadastro de veiculo pra autocomplete
</commit_message>
<xml_diff>
--- a/docs/features.xlsx
+++ b/docs/features.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Henrique\repos\fatec\fatecarona\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DACB13-A33C-4FE0-8CF9-E05666BE0C8E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB970A59-9BED-4988-965F-7D7A2CC33B61}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DC52FC83-1E62-41CF-BA03-5670C0B62DFB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>Senha arrumar</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>em vez de tirar o botão, agora da pra salvar sem carregar (acho que é interessante manter o botão carregar, se o usuario quiser ver a rota antes de salvar não podemos tirar essa opção dele, viola o feedback das heuristicas de nielsen)</t>
+  </si>
+  <si>
+    <t>complexo</t>
   </si>
 </sst>
 </file>
@@ -445,7 +448,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,10 +563,16 @@
       <c r="A16" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
+      </c>
+      <c r="D17" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>